<commit_message>
Added compute table codes fun w tests and mocks and cleaned up a bunch
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7592BD9-1BB8-469F-95A4-CFA5893A0424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DEBFDF-2569-44DE-9C65-AAD0CC3BB952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="4" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="3510" yWindow="1920" windowWidth="21375" windowHeight="13380" activeTab="8" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="32">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -109,6 +113,33 @@
   </si>
   <si>
     <t>umar--mz001--3--M</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>hgf</t>
+  </si>
+  <si>
+    <t>MZ001</t>
+  </si>
+  <si>
+    <t>MZ002</t>
+  </si>
+  <si>
+    <t>sd</t>
   </si>
 </sst>
 </file>
@@ -487,15 +518,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1217BD35-9581-47A9-A639-C8E3198F0BE2}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:H3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -518,10 +549,13 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -544,10 +578,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -570,6 +607,9 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -580,15 +620,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0752D223-8BC0-4B39-8EF7-4008561DDBA1}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -611,15 +651,18 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -631,15 +674,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714A082E-ABA1-4A37-A6B1-A1AE705D377F}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="A1:H5"/>
+      <selection activeCell="H6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -662,10 +705,13 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -688,10 +734,13 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -714,10 +763,13 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -737,10 +789,13 @@
         <v>1123</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -763,6 +818,9 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -773,15 +831,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366974F-121C-4CC0-AF7B-E602FAADC229}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -804,16 +862,19 @@
         <v>9</v>
       </c>
       <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -836,16 +897,19 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -868,16 +932,19 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -900,10 +967,13 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -926,6 +996,840 @@
         <v>16</v>
       </c>
       <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D37C2C-A139-4780-B623-69293A1F94FD}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A9FDAD-D17F-437D-B762-12251D8E7DDF}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BA6159-B412-4E20-B453-00B1ECFFD084}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C93FA7-BDD2-45F7-BA8D-0273E1A2895B}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1123</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add compute series code with tests and extra check
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DEBFDF-2569-44DE-9C65-AAD0CC3BB952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0B7B22-5EF3-4010-AAB6-4EAA414709D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1920" windowWidth="21375" windowHeight="13380" activeTab="8" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21375" windowHeight="13380" firstSheet="3" activeTab="4" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,10 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="36">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -140,6 +144,18 @@
   </si>
   <si>
     <t>sd</t>
+  </si>
+  <si>
+    <t>MZ003</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -516,6 +532,1131 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4068DA60-EF3C-43AC-8A88-419D111F5B87}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>1123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>1123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>1123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E3AED2-142E-4DCD-AC36-8B419CCF41B5}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>1123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>1123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>1123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C09B65F-FC58-4FCB-B473-8A9C02142A0D}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>1123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>1123</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>1123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3182FC-53FA-41F4-AA69-55ED7BAF537C}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1217BD35-9581-47A9-A639-C8E3198F0BE2}">
   <dimension ref="A1:I3"/>
@@ -833,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366974F-121C-4CC0-AF7B-E602FAADC229}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +2102,7 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>1123</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -990,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>1123</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
@@ -1545,8 +2686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C93FA7-BDD2-45F7-BA8D-0273E1A2895B}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add check for dimension level codes
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0B7B22-5EF3-4010-AAB6-4EAA414709D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D62F79-8A7E-42F2-947B-7C6378D62533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21375" windowHeight="13380" firstSheet="3" activeTab="4" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21375" windowHeight="13380" firstSheet="3" activeTab="13" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
     <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="40">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -156,6 +157,18 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>12--de32</t>
+  </si>
+  <si>
+    <t>93-B</t>
+  </si>
+  <si>
+    <t>testiram--123</t>
+  </si>
+  <si>
+    <t>B,D</t>
   </si>
 </sst>
 </file>
@@ -1455,7 +1468,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H6" sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,6 +1651,213 @@
       </c>
       <c r="F6" t="s">
         <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169EAB9B-7C2D-43A9-A495-1A2FA33D35A7}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>212</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -1974,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366974F-121C-4CC0-AF7B-E602FAADC229}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add prep and import table dimension fun with tests and mocks.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D62F79-8A7E-42F2-947B-7C6378D62533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7409DC2B-033B-409A-A09E-72F0A9814D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21375" windowHeight="13380" firstSheet="3" activeTab="13" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="5085" yWindow="1320" windowWidth="21375" windowHeight="13380" firstSheet="7" activeTab="16" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,10 @@
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
     <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
-    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId14"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId15"/>
+    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="50">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -169,6 +172,36 @@
   </si>
   <si>
     <t>B,D</t>
+  </si>
+  <si>
+    <t>dim1 -- dim2</t>
+  </si>
+  <si>
+    <t>dim3</t>
+  </si>
+  <si>
+    <t>sdfgs</t>
+  </si>
+  <si>
+    <t>4--2</t>
+  </si>
+  <si>
+    <t>3--2</t>
+  </si>
+  <si>
+    <t>dim1 -- dim2-- dim3</t>
+  </si>
+  <si>
+    <t>2--3--4</t>
+  </si>
+  <si>
+    <t>one -- two</t>
+  </si>
+  <si>
+    <t>one -- three</t>
+  </si>
+  <si>
+    <t>q--e--r</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1501,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A1:J6"/>
+      <selection activeCell="H6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,11 +1704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169EAB9B-7C2D-43A9-A495-1A2FA33D35A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE6A9D4-6372-49FB-8BAE-B16921CA8C75}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1762,7 @@
         <v>234</v>
       </c>
       <c r="F2">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -1760,6 +1793,213 @@
       <c r="E3">
         <v>1123</v>
       </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169EAB9B-7C2D-43A9-A495-1A2FA33D35A7}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>212</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
       <c r="F3" t="s">
         <v>36</v>
       </c>
@@ -1870,6 +2110,484 @@
       </c>
       <c r="J6" t="s">
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A20E50-4B87-4471-A5B3-AFBED5D6BF29}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>1123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2F88A-1C84-4ED4-83BE-9A3C90EB027B}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new check, w test
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7409DC2B-033B-409A-A09E-72F0A9814D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F5CAF5-8E5C-4A45-9F33-11F754468665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="1320" windowWidth="21375" windowHeight="13380" firstSheet="7" activeTab="16" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="5085" yWindow="1320" windowWidth="21375" windowHeight="13380" firstSheet="7" activeTab="17" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Sheet14" sheetId="14" r:id="rId15"/>
     <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
     <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet18" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="50">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -2360,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2F88A-1C84-4ED4-83BE-9A3C90EB027B}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,6 +2545,245 @@
       </c>
       <c r="F6" t="s">
         <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8375EF5-C7C3-4A3B-BF37-E1D6B90732E0}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Add prep and import fun for series table w tests and mocks.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F5CAF5-8E5C-4A45-9F33-11F754468665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD7466F-3F8C-4EC5-B0CE-46AC024DD66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="1320" windowWidth="21375" windowHeight="13380" firstSheet="7" activeTab="17" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="5085" yWindow="1320" windowWidth="21375" windowHeight="13380" activeTab="5" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,20 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
-    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
-    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
-    <sheet name="Sheet15" sheetId="15" r:id="rId14"/>
-    <sheet name="Sheet14" sheetId="14" r:id="rId15"/>
-    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
-    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
-    <sheet name="Sheet18" sheetId="18" r:id="rId18"/>
+    <sheet name="Sheet19" sheetId="19" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId11"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId12"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId13"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId16"/>
+    <sheet name="Sheet16" sheetId="16" r:id="rId17"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId18"/>
+    <sheet name="Sheet18" sheetId="18" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="54">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -203,6 +204,18 @@
   </si>
   <si>
     <t>q--e--r</t>
+  </si>
+  <si>
+    <t>UMAR--MZ001--234--M</t>
+  </si>
+  <si>
+    <t>UMAR--MZ001--1123--M</t>
+  </si>
+  <si>
+    <t>UMAR--MZ002--1--M</t>
+  </si>
+  <si>
+    <t>UMAR--MZ002--12--M</t>
   </si>
 </sst>
 </file>
@@ -580,6 +593,303 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C93FA7-BDD2-45F7-BA8D-0273E1A2895B}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1123</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4068DA60-EF3C-43AC-8A88-419D111F5B87}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -891,7 +1201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E3AED2-142E-4DCD-AC36-8B419CCF41B5}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -1194,7 +1504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C09B65F-FC58-4FCB-B473-8A9C02142A0D}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -1497,7 +1807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3182FC-53FA-41F4-AA69-55ED7BAF537C}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -1704,7 +2014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE6A9D4-6372-49FB-8BAE-B16921CA8C75}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -1911,7 +2221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169EAB9B-7C2D-43A9-A495-1A2FA33D35A7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2118,7 +2428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A20E50-4B87-4471-A5B3-AFBED5D6BF29}">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -2357,7 +2667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2F88A-1C84-4ED4-83BE-9A3C90EB027B}">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -2596,11 +2906,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8375EF5-C7C3-4A3B-BF37-E1D6B90732E0}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -3153,7 +3463,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3327,6 +3637,196 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B83DA9-8023-4E2F-9BB9-3CDC98B2C2BC}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D37C2C-A139-4780-B623-69293A1F94FD}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -3504,7 +4004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A9FDAD-D17F-437D-B762-12251D8E7DDF}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -3682,7 +4182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BA6159-B412-4E20-B453-00B1ECFFD084}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -3858,301 +4358,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C93FA7-BDD2-45F7-BA8D-0273E1A2895B}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1123</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>1123</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>1123</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>1123</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <v>1123</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add series name check and series name compute funs w tests.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD7466F-3F8C-4EC5-B0CE-46AC024DD66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27585E16-462B-4287-9591-2B20082CCF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="1320" windowWidth="21375" windowHeight="13380" activeTab="5" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="3" activeTab="6" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,19 +19,21 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet19" sheetId="19" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId9"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId11"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId12"/>
-    <sheet name="Sheet12" sheetId="12" r:id="rId13"/>
-    <sheet name="Sheet13" sheetId="13" r:id="rId14"/>
-    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
-    <sheet name="Sheet14" sheetId="14" r:id="rId16"/>
-    <sheet name="Sheet16" sheetId="16" r:id="rId17"/>
-    <sheet name="Sheet17" sheetId="17" r:id="rId18"/>
-    <sheet name="Sheet18" sheetId="18" r:id="rId19"/>
+    <sheet name="Sheet21" sheetId="21" r:id="rId7"/>
+    <sheet name="Sheet20" sheetId="20" r:id="rId8"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId9"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId10"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId11"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId12"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId13"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId14"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId15"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId16"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId17"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId18"/>
+    <sheet name="Sheet16" sheetId="16" r:id="rId19"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId20"/>
+    <sheet name="Sheet18" sheetId="18" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="61">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -216,6 +218,27 @@
   </si>
   <si>
     <t>UMAR--MZ002--12--M</t>
+  </si>
+  <si>
+    <t>kjh</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>wetr</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>cvb</t>
+  </si>
+  <si>
+    <t>gfj</t>
+  </si>
+  <si>
+    <t>fsfg</t>
   </si>
 </sst>
 </file>
@@ -593,6 +616,362 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A9FDAD-D17F-437D-B762-12251D8E7DDF}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BA6159-B412-4E20-B453-00B1ECFFD084}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1123</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C93FA7-BDD2-45F7-BA8D-0273E1A2895B}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -889,7 +1268,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4068DA60-EF3C-43AC-8A88-419D111F5B87}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -1201,7 +1580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E3AED2-142E-4DCD-AC36-8B419CCF41B5}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -1504,7 +1883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C09B65F-FC58-4FCB-B473-8A9C02142A0D}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -1807,12 +2186,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3182FC-53FA-41F4-AA69-55ED7BAF537C}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A1:XFD1048576"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,7 +2318,7 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
         <v>29</v>
@@ -1971,7 +2350,7 @@
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
@@ -2003,7 +2382,7 @@
         <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="J6" t="s">
         <v>30</v>
@@ -2014,7 +2393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE6A9D4-6372-49FB-8BAE-B16921CA8C75}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2221,7 +2600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169EAB9B-7C2D-43A9-A495-1A2FA33D35A7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2428,7 +2807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A20E50-4B87-4471-A5B3-AFBED5D6BF29}">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -2648,484 +3027,6 @@
       </c>
       <c r="F7" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2F88A-1C84-4ED4-83BE-9A3C90EB027B}">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>234</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>1123</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>1123</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8375EF5-C7C3-4A3B-BF37-E1D6B90732E0}">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>234</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>1123</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>1123</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
@@ -3247,6 +3148,484 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2F88A-1C84-4ED4-83BE-9A3C90EB027B}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8375EF5-C7C3-4A3B-BF37-E1D6B90732E0}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0752D223-8BC0-4B39-8EF7-4008561DDBA1}">
   <dimension ref="A1:I3"/>
@@ -3463,7 +3842,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,7 +3978,7 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3628,7 +4007,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3640,8 +4019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B83DA9-8023-4E2F-9BB9-3CDC98B2C2BC}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="A1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,7 +4156,7 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="J4" t="s">
         <v>30</v>
@@ -3812,7 +4191,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
@@ -3827,6 +4206,350 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A748DF8F-8B70-4971-9CD0-08EC8B8E2D69}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC72CF7A-589F-4078-8155-2E4A934DDB23}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D37C2C-A139-4780-B623-69293A1F94FD}">
   <dimension ref="A1:K5"/>
   <sheetViews>
@@ -4002,360 +4725,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A9FDAD-D17F-437D-B762-12251D8E7DDF}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1123</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BA6159-B412-4E20-B453-00B1ECFFD084}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1123</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Bumping up test coverage again
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEB838D-6248-4749-BB0C-3C1AFC2694B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B439791A-3131-402D-9F24-D2EA7993A292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="6" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="12" activeTab="22" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,23 +18,24 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet19" sheetId="19" r:id="rId6"/>
-    <sheet name="Sheet21" sheetId="21" r:id="rId7"/>
-    <sheet name="Sheet22" sheetId="22" r:id="rId8"/>
-    <sheet name="Sheet20" sheetId="20" r:id="rId9"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId10"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId11"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId12"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId13"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId14"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId15"/>
-    <sheet name="Sheet12" sheetId="12" r:id="rId16"/>
-    <sheet name="Sheet13" sheetId="13" r:id="rId17"/>
-    <sheet name="Sheet15" sheetId="15" r:id="rId18"/>
-    <sheet name="Sheet14" sheetId="14" r:id="rId19"/>
-    <sheet name="Sheet16" sheetId="16" r:id="rId20"/>
-    <sheet name="Sheet17" sheetId="17" r:id="rId21"/>
-    <sheet name="Sheet18" sheetId="18" r:id="rId22"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId14"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId15"/>
+    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
+    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
+    <sheet name="Sheet18" sheetId="18" r:id="rId18"/>
+    <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
+    <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
+    <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
+    <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
+    <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="61">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -617,837 +618,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D37C2C-A139-4780-B623-69293A1F94FD}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="A1:K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1123</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A9FDAD-D17F-437D-B762-12251D8E7DDF}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1123</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BA6159-B412-4E20-B453-00B1ECFFD084}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1123</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C93FA7-BDD2-45F7-BA8D-0273E1A2895B}">
-  <dimension ref="A1:K9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>1123</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>1123</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>1123</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>1123</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9">
-        <v>1123</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4068DA60-EF3C-43AC-8A88-419D111F5B87}">
   <dimension ref="A1:K9"/>
   <sheetViews>
@@ -1759,7 +929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E3AED2-142E-4DCD-AC36-8B419CCF41B5}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -2062,7 +1232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C09B65F-FC58-4FCB-B473-8A9C02142A0D}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -2365,7 +1535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3182FC-53FA-41F4-AA69-55ED7BAF537C}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2572,7 +1742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE6A9D4-6372-49FB-8BAE-B16921CA8C75}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2779,7 +1949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{169EAB9B-7C2D-43A9-A495-1A2FA33D35A7}">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -2979,6 +2149,913 @@
       </c>
       <c r="J6" t="s">
         <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A20E50-4B87-4471-A5B3-AFBED5D6BF29}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="A1:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>1123</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>1123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>1123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2F88A-1C84-4ED4-83BE-9A3C90EB027B}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="A1:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8375EF5-C7C3-4A3B-BF37-E1D6B90732E0}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B83DA9-8023-4E2F-9BB9-3CDC98B2C2BC}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3089,16 +3166,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A20E50-4B87-4471-A5B3-AFBED5D6BF29}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC72CF7A-589F-4078-8155-2E4A934DDB23}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:J7"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3129,8 +3206,11 @@
       <c r="J1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3144,10 +3224,10 @@
         <v>15</v>
       </c>
       <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
         <v>234</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -3158,11 +3238,8 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3176,10 +3253,10 @@
         <v>15</v>
       </c>
       <c r="E3">
-        <v>1123</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1123</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -3190,11 +3267,8 @@
       <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3202,16 +3276,16 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="E4">
-        <v>1123</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -3219,14 +3293,8 @@
       <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3234,92 +3302,22 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E5">
-        <v>1123</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6">
-        <v>1123</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7">
-        <v>1123</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3328,16 +3326,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F2F88A-1C84-4ED4-83BE-9A3C90EB027B}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A748DF8F-8B70-4971-9CD0-08EC8B8E2D69}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:J7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3368,8 +3366,11 @@
       <c r="J1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3383,10 +3384,10 @@
         <v>15</v>
       </c>
       <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
         <v>234</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -3400,8 +3401,11 @@
       <c r="J2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3415,25 +3419,25 @@
         <v>15</v>
       </c>
       <c r="E3">
-        <v>1123</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1123</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3447,10 +3451,10 @@
         <v>15</v>
       </c>
       <c r="E4">
-        <v>1123</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -3458,107 +3462,43 @@
       <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
       <c r="J4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
+      <c r="K5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3567,16 +3507,16 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8375EF5-C7C3-4A3B-BF37-E1D6B90732E0}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8400484-F015-4CC8-AAA2-63B3641AF1C6}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A5" sqref="A1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3607,8 +3547,11 @@
       <c r="J1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3622,10 +3565,10 @@
         <v>15</v>
       </c>
       <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
         <v>234</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -3639,8 +3582,11 @@
       <c r="J2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3654,25 +3600,25 @@
         <v>15</v>
       </c>
       <c r="E3">
-        <v>1123</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>1123</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3" t="s">
         <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -3686,10 +3632,10 @@
         <v>15</v>
       </c>
       <c r="E4">
-        <v>1123</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -3697,14 +3643,14 @@
       <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
       <c r="J4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3712,92 +3658,215 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B414E47-1533-4C62-8470-C7620D0CEB8F}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s">
-        <v>32</v>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -4195,11 +4264,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B83DA9-8023-4E2F-9BB9-3CDC98B2C2BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D37C2C-A139-4780-B623-69293A1F94FD}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="A1:K5"/>
+      <selection activeCell="H5" sqref="A1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4268,10 +4337,10 @@
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4303,10 +4372,10 @@
         <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4326,7 +4395,7 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1123</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -4335,13 +4404,7 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -4361,22 +4424,16 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>1123</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -4385,11 +4442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A748DF8F-8B70-4971-9CD0-08EC8B8E2D69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A9FDAD-D17F-437D-B762-12251D8E7DDF}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4458,10 +4515,10 @@
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4489,11 +4546,14 @@
       <c r="H3" t="s">
         <v>24</v>
       </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4504,7 +4564,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -4513,27 +4573,27 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1123</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -4542,22 +4602,16 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>1123</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -4566,11 +4620,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8400484-F015-4CC8-AAA2-63B3641AF1C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BA6159-B412-4E20-B453-00B1ECFFD084}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="A1:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4642,7 +4696,7 @@
         <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -4670,11 +4724,14 @@
       <c r="H3" t="s">
         <v>24</v>
       </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4694,19 +4751,16 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1123</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>52</v>
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -4717,7 +4771,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -4726,22 +4780,16 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>1123</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -4750,11 +4798,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC72CF7A-589F-4078-8155-2E4A934DDB23}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C93FA7-BDD2-45F7-BA8D-0273E1A2895B}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="M14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4822,6 +4870,12 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4851,6 +4905,12 @@
       <c r="I3" t="s">
         <v>18</v>
       </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4860,7 +4920,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -4869,13 +4929,16 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1123</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -4886,7 +4949,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -4895,13 +4958,135 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>12</v>
+        <v>1123</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1123</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added prep and import funs for series and series levels w tests and mocks
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B439791A-3131-402D-9F24-D2EA7993A292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C37B0C-5D12-4B89-A79C-664E015C7ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="12" activeTab="22" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="13" activeTab="18" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
     <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
     <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
+    <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="64">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -241,6 +242,15 @@
   </si>
   <si>
     <t>fsfg</t>
+  </si>
+  <si>
+    <t>4--3</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>dim1</t>
   </si>
 </sst>
 </file>
@@ -2161,7 +2171,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:J7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2639,7 +2649,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection sqref="A1:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B83DA9-8023-4E2F-9BB9-3CDC98B2C2BC}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="A1:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,10 +3006,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -3031,10 +3041,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -3694,7 +3704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B414E47-1533-4C62-8470-C7620D0CEB8F}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3867,6 +3877,245 @@
       </c>
       <c r="K5" t="s">
         <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633BBCBF-8B6F-441F-BB11-D7AE3E5728F8}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SOme test clean up for some reason
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C37B0C-5D12-4B89-A79C-664E015C7ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2027DFB-9C12-416A-BA06-89735AF95632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="13" activeTab="18" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="18900" windowHeight="11160" firstSheet="17" activeTab="24" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
     <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
     <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
+    <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="65">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -251,6 +252,9 @@
   </si>
   <si>
     <t>dim1</t>
+  </si>
+  <si>
+    <t>eurostat</t>
   </si>
 </sst>
 </file>
@@ -2887,7 +2891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83B83DA9-8023-4E2F-9BB9-3CDC98B2C2BC}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3180,7 +3184,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4123,6 +4127,166 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239DE753-F28E-49DB-8A2A-2FD2320A5E2A}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0752D223-8BC0-4B39-8EF7-4008561DDBA1}">
   <dimension ref="A1:I3"/>

</xml_diff>

<commit_message>
Add prep and import struc function and fix compute table fun, plus all the fcking mocks and tests cleaned up
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D087DA-77AF-442C-8507-CB16B773E6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5E61CD-FF4A-4963-863F-7DEFAB9C2977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2535" windowWidth="18900" windowHeight="11160" firstSheet="18" activeTab="24" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="18900" windowHeight="13440" firstSheet="18" activeTab="25" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
     <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
     <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
+    <sheet name="Sheet26" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="67">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -258,6 +259,9 @@
   </si>
   <si>
     <t>Založnik Maja</t>
+  </si>
+  <si>
+    <t>new name</t>
   </si>
 </sst>
 </file>
@@ -4134,8 +4138,168 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239DE753-F28E-49DB-8A2A-2FD2320A5E2A}">
   <dimension ref="A1:K5"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D1D3E-0AD5-4824-A2C5-6169AE99FB59}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5040,7 +5204,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5088,7 +5252,7 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -5123,7 +5287,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -5158,7 +5322,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -5218,7 +5382,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5266,7 +5430,7 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -5301,7 +5465,7 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -5336,7 +5500,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Add insert author and pull initials from db wiht checks, tests and mocks
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5E61CD-FF4A-4963-863F-7DEFAB9C2977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152CF8B0-9ACD-40CD-958F-D9F56AB5591E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="18900" windowHeight="13440" firstSheet="18" activeTab="25" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="18900" windowHeight="13440" firstSheet="19" activeTab="26" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
     <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
     <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
     <sheet name="Sheet26" sheetId="26" r:id="rId26"/>
+    <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="68">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -262,6 +263,9 @@
   </si>
   <si>
     <t>new name</t>
+  </si>
+  <si>
+    <t>Marko</t>
   </si>
 </sst>
 </file>
@@ -4298,8 +4302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D1D3E-0AD5-4824-A2C5-6169AE99FB59}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4429,6 +4433,166 @@
       </c>
       <c r="B5" t="s">
         <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE163D6B-D85C-4D07-A2D4-F401A5DBDE89}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Add some more checks for source and rewrite series code funciton w. tests and mocks.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152CF8B0-9ACD-40CD-958F-D9F56AB5591E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FCF27E-25AD-4445-A06A-1415197A6BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18900" windowHeight="13440" firstSheet="19" activeTab="26" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="25080" yWindow="-1245" windowWidth="19440" windowHeight="15150" firstSheet="12" activeTab="19" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,9 @@
     <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
     <sheet name="Sheet26" sheetId="26" r:id="rId26"/>
     <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
+    <sheet name="Sheet28" sheetId="28" r:id="rId28"/>
+    <sheet name="Sheet29" sheetId="29" r:id="rId29"/>
+    <sheet name="Sheet30" sheetId="30" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="72">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -266,6 +269,18 @@
   </si>
   <si>
     <t>Marko</t>
+  </si>
+  <si>
+    <t>umar, eurostat</t>
+  </si>
+  <si>
+    <t>umar,   imf</t>
+  </si>
+  <si>
+    <t>Investopedia, umar</t>
+  </si>
+  <si>
+    <t>umar, surs</t>
   </si>
 </sst>
 </file>
@@ -1564,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3182FC-53FA-41F4-AA69-55ED7BAF537C}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1619,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -1636,7 +1651,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -1668,7 +1683,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -1700,7 +1715,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -1732,7 +1747,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
@@ -1764,6 +1779,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2903,7 +2919,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,7 +2961,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -2980,7 +2996,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -3015,7 +3031,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -3050,7 +3066,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -3093,7 +3109,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,7 +3145,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -3158,7 +3174,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -3194,8 +3210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC72CF7A-589F-4078-8155-2E4A934DDB23}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3237,7 +3253,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -3266,7 +3282,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -3295,7 +3311,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -3321,7 +3337,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -4143,7 +4159,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4185,7 +4201,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -4214,7 +4230,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -4243,7 +4259,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -4269,7 +4285,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -4303,7 +4319,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4429,7 +4445,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -4462,8 +4478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE163D6B-D85C-4D07-A2D4-F401A5DBDE89}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,7 +4605,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
@@ -4611,6 +4627,309 @@
       </c>
       <c r="H5" t="s">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB59D9B5-92B7-4A04-91C6-C9DCA0A3095C}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7406A3DE-4250-4E2A-AC0C-3A86EF3E8AF6}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -4672,6 +4991,178 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D5206B-BA34-4B20-B22D-3607F6CB78B6}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714A082E-ABA1-4A37-A6B1-A1AE705D377F}">
   <dimension ref="A1:I5"/>
@@ -4834,7 +5325,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4876,7 +5367,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -4911,7 +5402,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -4946,7 +5437,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -4975,7 +5466,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Add extra check for metadata file
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FCF27E-25AD-4445-A06A-1415197A6BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121F390-6D9E-4927-94D2-5781DB1FC6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-1245" windowWidth="19440" windowHeight="15150" firstSheet="12" activeTab="19" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="1605" yWindow="1125" windowWidth="18900" windowHeight="13680" firstSheet="20" activeTab="21" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,28 @@
     <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
     <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
     <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
-    <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
-    <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
-    <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
-    <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
-    <sheet name="Sheet26" sheetId="26" r:id="rId26"/>
-    <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
-    <sheet name="Sheet28" sheetId="28" r:id="rId28"/>
-    <sheet name="Sheet29" sheetId="29" r:id="rId29"/>
-    <sheet name="Sheet30" sheetId="30" r:id="rId30"/>
+    <sheet name="Sheet31" sheetId="31" r:id="rId22"/>
+    <sheet name="Sheet32" sheetId="32" r:id="rId23"/>
+    <sheet name="Sheet33" sheetId="33" r:id="rId24"/>
+    <sheet name="Sheet34" sheetId="34" r:id="rId25"/>
+    <sheet name="Sheet35" sheetId="35" r:id="rId26"/>
+    <sheet name="Sheet36" sheetId="36" r:id="rId27"/>
+    <sheet name="Sheet37" sheetId="37" r:id="rId28"/>
+    <sheet name="Sheet38" sheetId="38" r:id="rId29"/>
+    <sheet name="Sheet39" sheetId="39" r:id="rId30"/>
+    <sheet name="Sheet40" sheetId="40" r:id="rId31"/>
+    <sheet name="Sheet41" sheetId="41" r:id="rId32"/>
+    <sheet name="Sheet42" sheetId="42" r:id="rId33"/>
+    <sheet name="Sheet43" sheetId="43" r:id="rId34"/>
+    <sheet name="Sheet22" sheetId="22" r:id="rId35"/>
+    <sheet name="Sheet23" sheetId="23" r:id="rId36"/>
+    <sheet name="Sheet24" sheetId="24" r:id="rId37"/>
+    <sheet name="Sheet25" sheetId="25" r:id="rId38"/>
+    <sheet name="Sheet26" sheetId="26" r:id="rId39"/>
+    <sheet name="Sheet27" sheetId="27" r:id="rId40"/>
+    <sheet name="Sheet28" sheetId="28" r:id="rId41"/>
+    <sheet name="Sheet29" sheetId="29" r:id="rId42"/>
+    <sheet name="Sheet30" sheetId="30" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="72">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -3210,7 +3223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC72CF7A-589F-4078-8155-2E4A934DDB23}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
@@ -3371,7 +3384,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3548,11 +3561,11 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8400484-F015-4CC8-AAA2-63B3641AF1C6}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364EA283-12CC-4FD0-A29F-71262A791AB0}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3592,1347 +3605,91 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B414E47-1533-4C62-8470-C7620D0CEB8F}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73A23F5-4BC3-4046-A874-C5A810B4AECC}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633BBCBF-8B6F-441F-BB11-D7AE3E5728F8}">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B8E97C-B274-42E7-A7A9-2C1ED49093C2}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>234</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>1123</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>1123</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239DE753-F28E-49DB-8A2A-2FD2320A5E2A}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B938AFB-337F-405F-8D83-F00DC4D4FA3B}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D1D3E-0AD5-4824-A2C5-6169AE99FB59}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA41685-F1B6-4B7C-A509-2E215B4BD834}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE163D6B-D85C-4D07-A2D4-F401A5DBDE89}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27F3B42-820F-48B4-AB0E-439D2B53C7B9}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB59D9B5-92B7-4A04-91C6-C9DCA0A3095C}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B14A1CC-7513-469C-8E12-A47DBF7D55ED}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:K5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7406A3DE-4250-4E2A-AC0C-3A86EF3E8AF6}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8659B1D8-80AC-47BF-8921-0AA009A41807}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4992,11 +3749,71 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D5206B-BA34-4B20-B22D-3607F6CB78B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3087DF1C-4D26-470F-9F41-195A037F8929}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF5970B-2D20-472A-8E59-600C280643D1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52292605-041B-4C20-A58E-E37A9F8A77D2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B133DA-A127-4827-B9D0-DC76775760B2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28406130-2E01-4153-9522-16EA8FD63691}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8400484-F015-4CC8-AAA2-63B3641AF1C6}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5038,7 +3855,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -5067,10 +3884,13 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -5093,12 +3913,12 @@
       <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
       <c r="J3" t="s">
         <v>27</v>
       </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -5108,7 +3928,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -5126,12 +3946,607 @@
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B414E47-1533-4C62-8470-C7620D0CEB8F}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633BBCBF-8B6F-441F-BB11-D7AE3E5728F8}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239DE753-F28E-49DB-8A2A-2FD2320A5E2A}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -5154,8 +4569,165 @@
       <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="J5" t="s">
-        <v>27</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D1D3E-0AD5-4824-A2C5-6169AE99FB59}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -5320,6 +4892,641 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE163D6B-D85C-4D07-A2D4-F401A5DBDE89}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB59D9B5-92B7-4A04-91C6-C9DCA0A3095C}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7406A3DE-4250-4E2A-AC0C-3A86EF3E8AF6}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D5206B-BA34-4B20-B22D-3607F6CB78B6}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366974F-121C-4CC0-AF7B-E602FAADC229}">
   <dimension ref="A1:K5"/>

</xml_diff>

<commit_message>
Add test for units w test
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/struct_tests.xlsx
+++ b/tests/testthat/testdata/struct_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\analysis\UMARfetchR\tests\testthat\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121F390-6D9E-4927-94D2-5781DB1FC6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B918ED1-4803-45A2-8A51-3A09D11B36C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="1125" windowWidth="18900" windowHeight="13680" firstSheet="20" activeTab="21" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
+    <workbookView xWindow="1515" yWindow="555" windowWidth="21345" windowHeight="14640" firstSheet="22" activeTab="30" xr2:uid="{1CDCE7F7-2EC9-457B-AE50-0EF67EB54273}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,28 +34,17 @@
     <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
     <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
     <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
-    <sheet name="Sheet31" sheetId="31" r:id="rId22"/>
-    <sheet name="Sheet32" sheetId="32" r:id="rId23"/>
-    <sheet name="Sheet33" sheetId="33" r:id="rId24"/>
-    <sheet name="Sheet34" sheetId="34" r:id="rId25"/>
-    <sheet name="Sheet35" sheetId="35" r:id="rId26"/>
-    <sheet name="Sheet36" sheetId="36" r:id="rId27"/>
-    <sheet name="Sheet37" sheetId="37" r:id="rId28"/>
-    <sheet name="Sheet38" sheetId="38" r:id="rId29"/>
-    <sheet name="Sheet39" sheetId="39" r:id="rId30"/>
-    <sheet name="Sheet40" sheetId="40" r:id="rId31"/>
-    <sheet name="Sheet41" sheetId="41" r:id="rId32"/>
-    <sheet name="Sheet42" sheetId="42" r:id="rId33"/>
-    <sheet name="Sheet43" sheetId="43" r:id="rId34"/>
-    <sheet name="Sheet22" sheetId="22" r:id="rId35"/>
-    <sheet name="Sheet23" sheetId="23" r:id="rId36"/>
-    <sheet name="Sheet24" sheetId="24" r:id="rId37"/>
-    <sheet name="Sheet25" sheetId="25" r:id="rId38"/>
-    <sheet name="Sheet26" sheetId="26" r:id="rId39"/>
-    <sheet name="Sheet27" sheetId="27" r:id="rId40"/>
-    <sheet name="Sheet28" sheetId="28" r:id="rId41"/>
-    <sheet name="Sheet29" sheetId="29" r:id="rId42"/>
-    <sheet name="Sheet30" sheetId="30" r:id="rId43"/>
+    <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
+    <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
+    <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
+    <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
+    <sheet name="Sheet26" sheetId="26" r:id="rId26"/>
+    <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
+    <sheet name="Sheet28" sheetId="28" r:id="rId28"/>
+    <sheet name="Sheet29" sheetId="29" r:id="rId29"/>
+    <sheet name="Sheet30" sheetId="30" r:id="rId30"/>
+    <sheet name="Sheet32" sheetId="44" r:id="rId31"/>
+    <sheet name="Sheet31" sheetId="31" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="76">
   <si>
     <t xml:space="preserve">one </t>
   </si>
@@ -294,6 +283,18 @@
   </si>
   <si>
     <t>umar, surs</t>
+  </si>
+  <si>
+    <t>bugi</t>
+  </si>
+  <si>
+    <t>wugi</t>
+  </si>
+  <si>
+    <t>umar, imf</t>
+  </si>
+  <si>
+    <t>2324fr</t>
   </si>
 </sst>
 </file>
@@ -3561,11 +3562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364EA283-12CC-4FD0-A29F-71262A791AB0}">
-  <dimension ref="A1:K1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8400484-F015-4CC8-AAA2-63B3641AF1C6}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,91 +3606,1347 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73A23F5-4BC3-4046-A874-C5A810B4AECC}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B414E47-1533-4C62-8470-C7620D0CEB8F}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B8E97C-B274-42E7-A7A9-2C1ED49093C2}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633BBCBF-8B6F-441F-BB11-D7AE3E5728F8}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>234</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1123</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>1123</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B938AFB-337F-405F-8D83-F00DC4D4FA3B}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239DE753-F28E-49DB-8A2A-2FD2320A5E2A}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA41685-F1B6-4B7C-A509-2E215B4BD834}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D1D3E-0AD5-4824-A2C5-6169AE99FB59}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27F3B42-820F-48B4-AB0E-439D2B53C7B9}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE163D6B-D85C-4D07-A2D4-F401A5DBDE89}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B14A1CC-7513-469C-8E12-A47DBF7D55ED}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB59D9B5-92B7-4A04-91C6-C9DCA0A3095C}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8659B1D8-80AC-47BF-8921-0AA009A41807}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7406A3DE-4250-4E2A-AC0C-3A86EF3E8AF6}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3749,71 +5006,11 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3087DF1C-4D26-470F-9F41-195A037F8929}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF5970B-2D20-472A-8E59-600C280643D1}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52292605-041B-4C20-A58E-E37A9F8A77D2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B133DA-A127-4827-B9D0-DC76775760B2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28406130-2E01-4153-9522-16EA8FD63691}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8400484-F015-4CC8-AAA2-63B3641AF1C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D5206B-BA34-4B20-B22D-3607F6CB78B6}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3855,7 +5052,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -3884,13 +5081,10 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -3913,12 +5107,12 @@
       <c r="H3" t="s">
         <v>22</v>
       </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
       <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3928,7 +5122,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -3946,21 +5140,18 @@
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -3977,14 +5168,8 @@
       <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
       <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3992,12 +5177,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B414E47-1533-4C62-8470-C7620D0CEB8F}">
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3E4AC-48E6-4E6F-9170-5B8947848866}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4039,7 +5224,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -4057,7 +5242,7 @@
         <v>234</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>
@@ -4068,19 +5253,16 @@
       <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
+      <c r="C3">
+        <v>3242</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -4092,27 +5274,27 @@
         <v>1123</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
         <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
       </c>
       <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -4130,21 +5312,18 @@
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -4161,14 +5340,8 @@
       <c r="H5" t="s">
         <v>22</v>
       </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
       <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -4176,251 +5349,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633BBCBF-8B6F-441F-BB11-D7AE3E5728F8}">
-  <dimension ref="A1:J7"/>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364EA283-12CC-4FD0-A29F-71262A791AB0}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>234</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>1123</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>1123</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239DE753-F28E-49DB-8A2A-2FD2320A5E2A}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4458,276 +5392,6 @@
       </c>
       <c r="K1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D1D3E-0AD5-4824-A2C5-6169AE99FB59}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4892,641 +5556,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE163D6B-D85C-4D07-A2D4-F401A5DBDE89}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB59D9B5-92B7-4A04-91C6-C9DCA0A3095C}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7406A3DE-4250-4E2A-AC0C-3A86EF3E8AF6}">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D5206B-BA34-4B20-B22D-3607F6CB78B6}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>234</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1123</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C366974F-121C-4CC0-AF7B-E602FAADC229}">
   <dimension ref="A1:K5"/>

</xml_diff>